<commit_message>
Swiftlink .CRT file support
</commit_message>
<xml_diff>
--- a/PCB/v0.2 archive/TeensyROM 0.2 pin-reg map.xlsx
+++ b/PCB/v0.2 archive/TeensyROM 0.2 pin-reg map.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\Commodore 64\Hardware\Expansion Port\TeensyROM\TeensyROM\PCB\v0.2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyData\Geek Stuff\Projects\Commodore 64\Hardware\Expansion Port\TeensyROM\TeensyROM\PCB\v0.2 archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A61B238-A4A4-470D-A037-62463FBAEE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15D16F4-3E8A-4857-81F3-5285DD6967FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Exp Port" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Pin Map'!$B$2:$O$59</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Pin Map'!$B$2:$P$59</definedName>
   </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="249">
   <si>
     <t>Teensy 4.0</t>
   </si>
@@ -775,6 +775,18 @@
   </si>
   <si>
     <t>Debug/Spare</t>
+  </si>
+  <si>
+    <t>Using?</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>No, but may</t>
   </si>
 </sst>
 </file>
@@ -801,7 +813,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -847,6 +859,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -941,7 +965,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -993,7 +1017,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1417,11 +1446,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{438729BD-DE3A-4627-A7A2-2FBBC7D246EF}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B1:O59"/>
+  <dimension ref="B1:P59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M37" sqref="M37"/>
+      <pane ySplit="2" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1430,14 +1459,14 @@
     <col min="2" max="5" width="11.109375" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="11.109375" customWidth="1"/>
     <col min="7" max="8" width="8.33203125" customWidth="1"/>
-    <col min="9" max="10" width="11.109375" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" style="17" customWidth="1"/>
-    <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.44140625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="26.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="11.109375" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" style="17" customWidth="1"/>
+    <col min="14" max="14" width="21" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.44140625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="26.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1453,13 +1482,16 @@
       <c r="J1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="15"/>
-      <c r="L1" s="10"/>
+      <c r="K1" s="30" t="s">
+        <v>245</v>
+      </c>
+      <c r="L1" s="15"/>
       <c r="M1" s="10"/>
-      <c r="N1" s="7"/>
+      <c r="N1" s="10"/>
       <c r="O1" s="7"/>
-    </row>
-    <row r="2" spans="2:15" s="20" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="P1" s="7"/>
+    </row>
+    <row r="2" spans="2:16" s="20" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
         <v>3</v>
       </c>
@@ -1487,23 +1519,24 @@
       <c r="J2" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="31"/>
+      <c r="L2" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="L2" s="25" t="s">
+      <c r="M2" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="M2" s="25" t="s">
+      <c r="N2" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="O2" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="26" t="s">
+      <c r="P2" s="26" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" s="27" t="s">
         <v>36</v>
       </c>
@@ -1531,19 +1564,22 @@
       <c r="J3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K3" s="16"/>
-      <c r="L3" s="1" t="s">
+      <c r="K3" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="L3" s="16"/>
+      <c r="M3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O3" s="18"/>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P3" s="18"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" s="27" t="s">
         <v>36</v>
       </c>
@@ -1565,27 +1601,30 @@
       <c r="H4" s="1">
         <v>1</v>
       </c>
-      <c r="I4" s="29" t="s">
+      <c r="I4" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="16"/>
-      <c r="L4" s="1" t="s">
+      <c r="K4" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="L4" s="16"/>
+      <c r="M4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O4" s="18" t="s">
+      <c r="P4" s="18" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>39</v>
       </c>
@@ -1613,19 +1652,22 @@
       <c r="J5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K5" s="16"/>
-      <c r="L5" s="1" t="s">
+      <c r="K5" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="L5" s="16"/>
+      <c r="M5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O5" s="1"/>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P5" s="1"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>39</v>
       </c>
@@ -1653,19 +1695,22 @@
       <c r="J6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K6" s="16"/>
-      <c r="L6" s="1" t="s">
+      <c r="K6" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="L6" s="16"/>
+      <c r="M6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="O6" s="1"/>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P6" s="1"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>39</v>
       </c>
@@ -1693,19 +1738,22 @@
       <c r="J7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K7" s="16"/>
-      <c r="L7" s="1" t="s">
+      <c r="K7" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="L7" s="16"/>
+      <c r="M7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="O7" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="O7" s="1"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P7" s="1"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>39</v>
       </c>
@@ -1727,25 +1775,28 @@
       <c r="H8" s="1">
         <v>5</v>
       </c>
-      <c r="I8" s="29" t="s">
+      <c r="I8" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K8" s="16"/>
-      <c r="L8" s="1" t="s">
+      <c r="K8" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="L8" s="16"/>
+      <c r="M8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P8" s="1"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>37</v>
       </c>
@@ -1773,23 +1824,26 @@
       <c r="J9" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="K9" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="L9" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="M9" s="9" t="s">
+      <c r="N9" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>37</v>
       </c>
@@ -1817,19 +1871,22 @@
       <c r="J10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="16"/>
-      <c r="L10" s="1" t="s">
+      <c r="K10" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="L10" s="16"/>
+      <c r="M10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O10" s="1"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P10" s="1"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>37</v>
       </c>
@@ -1857,19 +1914,22 @@
       <c r="J11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="16"/>
-      <c r="L11" s="1" t="s">
+      <c r="K11" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="L11" s="16"/>
+      <c r="M11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="N11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="O11" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O11" s="1"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P11" s="1"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>37</v>
       </c>
@@ -1897,21 +1957,24 @@
       <c r="J12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="K12" s="16">
+      <c r="K12" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="L12" s="16">
         <v>9</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M12" s="9" t="s">
+      <c r="N12" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="O12" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="O12" s="1"/>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P12" s="1"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>37</v>
       </c>
@@ -1939,19 +2002,22 @@
       <c r="J13" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K13" s="16"/>
-      <c r="L13" s="1" t="s">
+      <c r="K13" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="L13" s="16"/>
+      <c r="M13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="O13" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O13" s="1"/>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P13" s="1"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>37</v>
       </c>
@@ -1979,19 +2045,22 @@
       <c r="J14" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="K14" s="16"/>
-      <c r="L14" s="1" t="s">
+      <c r="K14" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="L14" s="16"/>
+      <c r="M14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="O14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>37</v>
       </c>
@@ -2019,19 +2088,22 @@
       <c r="J15" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K15" s="16"/>
-      <c r="L15" s="1" t="s">
+      <c r="K15" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="L15" s="16"/>
+      <c r="M15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="O15" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P15" s="1"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>37</v>
       </c>
@@ -2059,21 +2131,24 @@
       <c r="J16" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K16" s="16"/>
-      <c r="L16" s="1" t="s">
+      <c r="K16" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="L16" s="16"/>
+      <c r="M16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="N16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="O16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O16" s="1" t="s">
+      <c r="P16" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
         <v>36</v>
       </c>
@@ -2101,19 +2176,22 @@
       <c r="J17" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="K17" s="16"/>
-      <c r="L17" s="1" t="s">
+      <c r="K17" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L17" s="16"/>
+      <c r="M17" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="O17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O17" s="1"/>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P17" s="1"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
@@ -2141,19 +2219,22 @@
       <c r="J18" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="K18" s="16"/>
-      <c r="L18" s="1" t="s">
+      <c r="K18" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L18" s="16"/>
+      <c r="M18" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="N18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="O18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P18" s="1"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>36</v>
       </c>
@@ -2181,19 +2262,22 @@
       <c r="J19" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="K19" s="16"/>
-      <c r="L19" s="1" t="s">
+      <c r="K19" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L19" s="16"/>
+      <c r="M19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="N19" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N19" s="1" t="s">
+      <c r="O19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O19" s="1"/>
-    </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
         <v>36</v>
       </c>
@@ -2221,19 +2305,22 @@
       <c r="J20" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="K20" s="16"/>
-      <c r="L20" s="1" t="s">
+      <c r="K20" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L20" s="16"/>
+      <c r="M20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="N20" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="O20" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O20" s="1"/>
-    </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>36</v>
       </c>
@@ -2261,19 +2348,22 @@
       <c r="J21" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="K21" s="16"/>
-      <c r="L21" s="1" t="s">
+      <c r="K21" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L21" s="16"/>
+      <c r="M21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="N21" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N21" s="1" t="s">
+      <c r="O21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O21" s="1"/>
-    </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P21" s="1"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>36</v>
       </c>
@@ -2301,19 +2391,22 @@
       <c r="J22" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="K22" s="16"/>
-      <c r="L22" s="1" t="s">
+      <c r="K22" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L22" s="16"/>
+      <c r="M22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="N22" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N22" s="1" t="s">
+      <c r="O22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O22" s="1"/>
-    </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P22" s="1"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>36</v>
       </c>
@@ -2341,19 +2434,22 @@
       <c r="J23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K23" s="16"/>
-      <c r="L23" s="1" t="s">
+      <c r="K23" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L23" s="16"/>
+      <c r="M23" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="N23" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N23" s="1" t="s">
+      <c r="O23" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="O23" s="1"/>
-    </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P23" s="1"/>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>36</v>
       </c>
@@ -2381,19 +2477,22 @@
       <c r="J24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K24" s="16"/>
-      <c r="L24" s="1" t="s">
+      <c r="K24" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L24" s="16"/>
+      <c r="M24" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="N24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N24" s="1" t="s">
+      <c r="O24" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="O24" s="1"/>
-    </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P24" s="1"/>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
         <v>36</v>
       </c>
@@ -2421,19 +2520,22 @@
       <c r="J25" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="K25" s="16"/>
-      <c r="L25" s="1" t="s">
+      <c r="K25" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L25" s="16"/>
+      <c r="M25" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="N25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N25" s="1" t="s">
+      <c r="O25" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="O25" s="1"/>
-    </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P25" s="1"/>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>36</v>
       </c>
@@ -2461,19 +2563,22 @@
       <c r="J26" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="K26" s="16"/>
-      <c r="L26" s="1" t="s">
+      <c r="K26" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L26" s="16"/>
+      <c r="M26" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="N26" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N26" s="1" t="s">
+      <c r="O26" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="O26" s="1"/>
-    </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P26" s="1"/>
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
         <v>36</v>
       </c>
@@ -2501,23 +2606,26 @@
       <c r="J27" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="K27" s="16">
+      <c r="K27" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="L27" s="16">
         <v>4</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="M27" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="M27" s="9" t="s">
+      <c r="N27" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="N27" s="1" t="s">
+      <c r="O27" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="O27" s="1" t="s">
+      <c r="P27" s="1" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>36</v>
       </c>
@@ -2545,23 +2653,26 @@
       <c r="J28" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="K28" s="16" t="s">
+      <c r="K28" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="L28" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="L28" s="1" t="s">
+      <c r="M28" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="M28" s="9" t="s">
+      <c r="N28" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="N28" s="1" t="s">
+      <c r="O28" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="O28" s="1" t="s">
+      <c r="P28" s="1" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>36</v>
       </c>
@@ -2589,19 +2700,22 @@
       <c r="J29" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="K29" s="16"/>
-      <c r="L29" s="1" t="s">
+      <c r="K29" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="L29" s="16"/>
+      <c r="M29" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="N29" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N29" s="1" t="s">
+      <c r="O29" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="O29" s="1"/>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P29" s="1"/>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>36</v>
       </c>
@@ -2629,19 +2743,22 @@
       <c r="J30" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="K30" s="16"/>
-      <c r="L30" s="1" t="s">
+      <c r="K30" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="L30" s="16"/>
+      <c r="M30" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="N30" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N30" s="1" t="s">
+      <c r="O30" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="O30" s="1"/>
-    </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P30" s="1"/>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>38</v>
       </c>
@@ -2669,23 +2786,26 @@
       <c r="J31" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K31" s="16">
+      <c r="K31" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="L31" s="16">
         <v>6</v>
       </c>
-      <c r="L31" s="1" t="s">
+      <c r="M31" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M31" s="1" t="s">
+      <c r="N31" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N31" s="1" t="s">
+      <c r="O31" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="O31" s="1" t="s">
+      <c r="P31" s="1" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>39</v>
       </c>
@@ -2713,19 +2833,22 @@
       <c r="J32" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="K32" s="16"/>
-      <c r="L32" s="1" t="s">
+      <c r="K32" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="L32" s="16"/>
+      <c r="M32" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M32" s="1" t="s">
+      <c r="N32" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N32" s="1" t="s">
+      <c r="O32" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="O32" s="1"/>
-    </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P32" s="1"/>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>38</v>
       </c>
@@ -2753,21 +2876,24 @@
       <c r="J33" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="K33" s="16">
+      <c r="K33" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="L33" s="16">
         <v>13</v>
       </c>
-      <c r="L33" s="1" t="s">
+      <c r="M33" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M33" s="9" t="s">
+      <c r="N33" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="N33" s="1" t="s">
+      <c r="O33" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="O33" s="1"/>
-    </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P33" s="1"/>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
         <v>38</v>
       </c>
@@ -2795,17 +2921,20 @@
       <c r="J34" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="K34" s="16"/>
-      <c r="L34" s="1" t="s">
+      <c r="K34" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="L34" s="16"/>
+      <c r="M34" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M34" s="1" t="s">
+      <c r="N34" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="N34" s="1"/>
       <c r="O34" s="1"/>
-    </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P34" s="1"/>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
         <v>37</v>
       </c>
@@ -2833,21 +2962,24 @@
       <c r="J35" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K35" s="16">
+      <c r="K35" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="L35" s="16">
         <v>8</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="M35" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M35" s="9" t="s">
+      <c r="N35" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="N35" s="1" t="s">
+      <c r="O35" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="O35" s="1"/>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P35" s="1"/>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>39</v>
       </c>
@@ -2869,23 +3001,26 @@
       <c r="H36" s="1">
         <v>33</v>
       </c>
-      <c r="I36" s="29" t="s">
+      <c r="I36" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="K36" s="16"/>
-      <c r="L36" s="1" t="s">
+      <c r="K36" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="L36" s="16"/>
+      <c r="M36" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M36" s="29" t="s">
+      <c r="N36" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="N36" s="1"/>
       <c r="O36" s="1"/>
-    </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P36" s="1"/>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>38</v>
       </c>
@@ -2913,17 +3048,20 @@
       <c r="J37" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="K37" s="16"/>
-      <c r="L37" s="1" t="s">
+      <c r="K37" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="L37" s="16"/>
+      <c r="M37" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M37" s="1" t="s">
+      <c r="N37" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="N37" s="1"/>
       <c r="O37" s="1"/>
-    </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P37" s="1"/>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
         <v>38</v>
       </c>
@@ -2945,25 +3083,28 @@
       <c r="H38" s="1">
         <v>35</v>
       </c>
-      <c r="I38" s="29" t="s">
+      <c r="I38" s="1" t="s">
         <v>43</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K38" s="16"/>
-      <c r="L38" s="1" t="s">
+      <c r="K38" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="L38" s="16"/>
+      <c r="M38" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M38" s="1" t="s">
+      <c r="N38" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="N38" s="1" t="s">
+      <c r="O38" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O38" s="1"/>
-    </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P38" s="1"/>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
         <v>38</v>
       </c>
@@ -2991,19 +3132,22 @@
       <c r="J39" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K39" s="16"/>
-      <c r="L39" s="1" t="s">
+      <c r="K39" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="L39" s="16"/>
+      <c r="M39" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M39" s="1" t="s">
+      <c r="N39" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N39" s="1" t="s">
+      <c r="O39" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O39" s="1"/>
-    </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P39" s="1"/>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
         <v>38</v>
       </c>
@@ -3031,19 +3175,22 @@
       <c r="J40" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="K40" s="16"/>
-      <c r="L40" s="1" t="s">
+      <c r="K40" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="L40" s="16"/>
+      <c r="M40" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M40" s="1" t="s">
+      <c r="N40" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N40" s="1" t="s">
+      <c r="O40" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O40" s="1"/>
-    </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P40" s="1"/>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
         <v>38</v>
       </c>
@@ -3071,19 +3218,22 @@
       <c r="J41" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K41" s="16"/>
-      <c r="L41" s="1" t="s">
+      <c r="K41" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L41" s="16"/>
+      <c r="M41" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M41" s="1" t="s">
+      <c r="N41" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N41" s="1" t="s">
+      <c r="O41" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="O41" s="1"/>
-    </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P41" s="1"/>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>38</v>
       </c>
@@ -3111,19 +3261,22 @@
       <c r="J42" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="K42" s="16"/>
-      <c r="L42" s="1" t="s">
+      <c r="K42" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="L42" s="16"/>
+      <c r="M42" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M42" s="1" t="s">
+      <c r="N42" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N42" s="1" t="s">
+      <c r="O42" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="O42" s="1"/>
-    </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P42" s="1"/>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -3143,19 +3296,22 @@
       <c r="J43" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="K43" s="16"/>
-      <c r="L43" s="1" t="s">
+      <c r="K43" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L43" s="16"/>
+      <c r="M43" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M43" s="1" t="s">
+      <c r="N43" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N43" s="1" t="s">
+      <c r="O43" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O43" s="1"/>
-    </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P43" s="1"/>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -3175,19 +3331,22 @@
       <c r="J44" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="K44" s="16"/>
-      <c r="L44" s="1" t="s">
+      <c r="K44" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L44" s="16"/>
+      <c r="M44" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M44" s="1" t="s">
+      <c r="N44" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N44" s="1" t="s">
+      <c r="O44" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="O44" s="1"/>
-    </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P44" s="1"/>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -3205,15 +3364,18 @@
         <v>28</v>
       </c>
       <c r="J45" s="1"/>
-      <c r="K45" s="16"/>
-      <c r="L45" s="1"/>
+      <c r="K45" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L45" s="16"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
-      <c r="O45" s="1" t="s">
+      <c r="O45" s="1"/>
+      <c r="P45" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -3231,15 +3393,18 @@
         <v>28</v>
       </c>
       <c r="J46" s="1"/>
-      <c r="K46" s="16"/>
-      <c r="L46" s="1"/>
+      <c r="K46" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L46" s="16"/>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
-      <c r="O46" s="1" t="s">
+      <c r="O46" s="1"/>
+      <c r="P46" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -3257,15 +3422,18 @@
         <v>28</v>
       </c>
       <c r="J47" s="1"/>
-      <c r="K47" s="16"/>
-      <c r="L47" s="1"/>
+      <c r="K47" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L47" s="16"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
-      <c r="O47" s="1" t="s">
+      <c r="O47" s="1"/>
+      <c r="P47" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -3283,15 +3451,18 @@
         <v>28</v>
       </c>
       <c r="J48" s="1"/>
-      <c r="K48" s="16"/>
-      <c r="L48" s="1"/>
+      <c r="K48" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L48" s="16"/>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
-      <c r="O48" s="1" t="s">
+      <c r="O48" s="1"/>
+      <c r="P48" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -3309,15 +3480,18 @@
         <v>28</v>
       </c>
       <c r="J49" s="1"/>
-      <c r="K49" s="16"/>
-      <c r="L49" s="1"/>
+      <c r="K49" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L49" s="16"/>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
-      <c r="O49" s="1" t="s">
+      <c r="O49" s="1"/>
+      <c r="P49" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -3335,15 +3509,18 @@
         <v>28</v>
       </c>
       <c r="J50" s="1"/>
-      <c r="K50" s="16"/>
-      <c r="L50" s="1"/>
+      <c r="K50" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L50" s="16"/>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
-      <c r="O50" s="1" t="s">
+      <c r="O50" s="1"/>
+      <c r="P50" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -3361,15 +3538,18 @@
         <v>28</v>
       </c>
       <c r="J51" s="1"/>
-      <c r="K51" s="16"/>
-      <c r="L51" s="1"/>
+      <c r="K51" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="L51" s="16"/>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
-      <c r="O51" s="1" t="s">
+      <c r="O51" s="1"/>
+      <c r="P51" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -3387,15 +3567,18 @@
         <v>28</v>
       </c>
       <c r="J52" s="1"/>
-      <c r="K52" s="16"/>
-      <c r="L52" s="1"/>
+      <c r="K52" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="L52" s="16"/>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
-      <c r="O52" s="1" t="s">
+      <c r="O52" s="1"/>
+      <c r="P52" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -3413,15 +3596,18 @@
         <v>28</v>
       </c>
       <c r="J53" s="1"/>
-      <c r="K53" s="16"/>
-      <c r="L53" s="1"/>
+      <c r="K53" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="L53" s="16"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
-      <c r="O53" s="1" t="s">
+      <c r="O53" s="1"/>
+      <c r="P53" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -3439,15 +3625,18 @@
         <v>28</v>
       </c>
       <c r="J54" s="1"/>
-      <c r="K54" s="16"/>
-      <c r="L54" s="1"/>
+      <c r="K54" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="L54" s="16"/>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
-      <c r="O54" s="1" t="s">
+      <c r="O54" s="1"/>
+      <c r="P54" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -3465,15 +3654,18 @@
         <v>28</v>
       </c>
       <c r="J55" s="1"/>
-      <c r="K55" s="16"/>
-      <c r="L55" s="1"/>
+      <c r="K55" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="L55" s="16"/>
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
-      <c r="O55" s="1" t="s">
+      <c r="O55" s="1"/>
+      <c r="P55" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -3491,15 +3683,18 @@
         <v>28</v>
       </c>
       <c r="J56" s="1"/>
-      <c r="K56" s="16"/>
-      <c r="L56" s="1"/>
+      <c r="K56" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="L56" s="16"/>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
-      <c r="O56" s="1" t="s">
+      <c r="O56" s="1"/>
+      <c r="P56" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -3517,15 +3712,18 @@
         <v>28</v>
       </c>
       <c r="J57" s="1"/>
-      <c r="K57" s="16"/>
-      <c r="L57" s="1"/>
+      <c r="K57" s="29" t="s">
+        <v>247</v>
+      </c>
+      <c r="L57" s="16"/>
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
-      <c r="O57" s="1" t="s">
+      <c r="O57" s="1"/>
+      <c r="P57" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B58" s="28"/>
       <c r="C58" s="28"/>
       <c r="D58" s="28"/>
@@ -3545,19 +3743,22 @@
       <c r="J58" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="K58" s="16" t="s">
+      <c r="K58" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L58" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="L58" s="1" t="s">
+      <c r="M58" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="M58" s="1"/>
-      <c r="N58" s="1" t="s">
+      <c r="N58" s="1"/>
+      <c r="O58" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="O58" s="1"/>
-    </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="P58" s="1"/>
+    </row>
+    <row r="59" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B59" s="28"/>
       <c r="C59" s="28"/>
       <c r="D59" s="28"/>
@@ -3577,23 +3778,26 @@
       <c r="J59" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="K59" s="16" t="s">
+      <c r="K59" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="L59" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="L59" s="1" t="s">
+      <c r="M59" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="M59" s="1"/>
-      <c r="N59" s="1" t="s">
+      <c r="N59" s="1"/>
+      <c r="O59" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="O59" s="1" t="s">
+      <c r="P59" s="1" t="s">
         <v>217</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B2:O59" xr:uid="{438729BD-DE3A-4627-A7A2-2FBBC7D246EF}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:O59">
+  <autoFilter ref="B2:P59" xr:uid="{438729BD-DE3A-4627-A7A2-2FBBC7D246EF}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:P59">
       <sortCondition ref="H2:H59"/>
     </sortState>
   </autoFilter>
@@ -3601,32 +3805,32 @@
     <sortCondition ref="D5:D59"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="B1:B44">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="GPIO8">
+      <formula>NOT(ISERROR(SEARCH("GPIO8",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="GPIO7">
+      <formula>NOT(ISERROR(SEARCH("GPIO7",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="11" operator="containsText" text="GPIO9">
+      <formula>NOT(ISERROR(SEARCH("GPIO9",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="12" operator="containsText" text="GPIO6">
+      <formula>NOT(ISERROR(SEARCH("GPIO6",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="7" priority="13" operator="containsText" text="GPIO8">
+    <cfRule type="containsText" dxfId="3" priority="13" operator="containsText" text="GPIO8">
       <formula>NOT(ISERROR(SEARCH("GPIO8",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="14" operator="containsText" text="GPIO7">
+    <cfRule type="containsText" dxfId="2" priority="14" operator="containsText" text="GPIO7">
       <formula>NOT(ISERROR(SEARCH("GPIO7",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="15" operator="containsText" text="GPIO9">
+    <cfRule type="containsText" dxfId="1" priority="15" operator="containsText" text="GPIO9">
       <formula>NOT(ISERROR(SEARCH("GPIO9",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="16" operator="containsText" text="GPIO6">
+    <cfRule type="containsText" dxfId="0" priority="16" operator="containsText" text="GPIO6">
       <formula>NOT(ISERROR(SEARCH("GPIO6",F1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B44">
-    <cfRule type="containsText" dxfId="3" priority="9" operator="containsText" text="GPIO8">
-      <formula>NOT(ISERROR(SEARCH("GPIO8",B1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="10" operator="containsText" text="GPIO7">
-      <formula>NOT(ISERROR(SEARCH("GPIO7",B1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="11" operator="containsText" text="GPIO9">
-      <formula>NOT(ISERROR(SEARCH("GPIO9",B1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="12" operator="containsText" text="GPIO6">
-      <formula>NOT(ISERROR(SEARCH("GPIO6",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>